<commit_message>
docs(documentation): add new documentation fonctionnelle et technique
</commit_message>
<xml_diff>
--- a/documentation/dossier_fonctionnel/backlog.xlsx
+++ b/documentation/dossier_fonctionnel/backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\bts1\piscine3\documents\dossier_fonctionnel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iwn\bts2\livequestion\documentation\dossier_fonctionnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CA6738-22B8-453D-8383-BAF087E6D439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D787EB-A20B-4926-A63E-FC472AECB68F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="750" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>fonctionnalité</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>affiche l'ensemble des questions</t>
   </si>
@@ -39,9 +33,6 @@
     <t>ajouter question</t>
   </si>
   <si>
-    <t>ajouter une question en base de données</t>
-  </si>
-  <si>
     <t>modification profil</t>
   </si>
   <si>
@@ -75,9 +66,6 @@
     <t>modification question</t>
   </si>
   <si>
-    <t>modifier une question</t>
-  </si>
-  <si>
     <t>espace administrateur</t>
   </si>
   <si>
@@ -90,12 +78,6 @@
     <t>question uniquement visible par ses amis</t>
   </si>
   <si>
-    <t>supprimer une question</t>
-  </si>
-  <si>
-    <t>permet de supprimer définitivement une question</t>
-  </si>
-  <si>
     <t>supprimer utilisateur</t>
   </si>
   <si>
@@ -109,6 +91,78 @@
   </si>
   <si>
     <t>flux de questions</t>
+  </si>
+  <si>
+    <t>supprimer question</t>
+  </si>
+  <si>
+    <t>supprimer une question stockée en base de données</t>
+  </si>
+  <si>
+    <t>ajouter une question stockée en base de données</t>
+  </si>
+  <si>
+    <t>modifier une question stockée en base de données</t>
+  </si>
+  <si>
+    <t>rechercher question</t>
+  </si>
+  <si>
+    <t>répondre question</t>
+  </si>
+  <si>
+    <t>rechercher une question par son titre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">répondre à une question </t>
+  </si>
+  <si>
+    <t>ajouter ami</t>
+  </si>
+  <si>
+    <t>ajouter un utilisateur en ami</t>
+  </si>
+  <si>
+    <t>supprimer ami</t>
+  </si>
+  <si>
+    <t>supprimer un utilisateur en ami</t>
+  </si>
+  <si>
+    <t>Fonctionnalité</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>supprimer réponse</t>
+  </si>
+  <si>
+    <t>supprimer sa réponse à une question</t>
+  </si>
+  <si>
+    <t>voir ami</t>
+  </si>
+  <si>
+    <t>voir la liste de ses amis</t>
+  </si>
+  <si>
+    <t>aimer question</t>
+  </si>
+  <si>
+    <t>aimer une question</t>
+  </si>
+  <si>
+    <t>retirer aime question</t>
+  </si>
+  <si>
+    <t>retirer le j'aime d'une question</t>
+  </si>
+  <si>
+    <t>je n'aime pas question</t>
+  </si>
+  <si>
+    <t>ne pas aimer une question</t>
   </si>
 </sst>
 </file>
@@ -426,80 +480,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -512,42 +566,114 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>